<commit_message>
fixed bugs on reporting.py and master log
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,18 +15,189 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+  <si>
+    <t>January 2017</t>
+  </si>
+  <si>
+    <t>saeccffrgeaa Gary Tsai 2016-08-26 16:50:26.807392</t>
+  </si>
+  <si>
+    <t>saeccffrgea  2016-08-26 16:52:18.777307</t>
+  </si>
+  <si>
+    <t>05 17:50&gt;&gt;&gt; CFD893A460 Gary Tsai</t>
+  </si>
+  <si>
+    <t>05 18:01&gt;&gt;&gt; 0FD8AC7AC0 Alfonse D'Elia</t>
+  </si>
+  <si>
+    <t>06 09:36&gt;&gt;&gt; 0FD89CD000 David Schachner</t>
+  </si>
+  <si>
+    <t>09 10:26&gt;&gt;&gt; 0FD8AF13C0 Rondell Holland</t>
+  </si>
+  <si>
+    <t>10 08:59&gt;&gt;&gt; CFD88517C0 Joseph Giordano</t>
+  </si>
+  <si>
+    <t>10 10:10&gt;&gt;&gt; CFD893A460 Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 10:36&gt;&gt;&gt; 0FD89CD000 David Schachner</t>
+  </si>
+  <si>
+    <t>10 11:31&gt;&gt;&gt; CFD893A460 Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 12:43&gt;&gt;&gt; 8FD8A841E0 Sujay Bhaskar KashYap</t>
+  </si>
+  <si>
+    <t>10 13:06&gt;&gt;&gt; CFD893A460 Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 13:08&gt;&gt;&gt; CFD893A460 Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:10&gt;&gt;&gt; 0FD8ABF6C0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:11&gt;&gt;&gt; 0FD8ABF6C0 </t>
+  </si>
+  <si>
+    <t>10 13:19&gt;&gt;&gt; 0FD8AD9C60 everton mendozaholmes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:25&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 13:29&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:30&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 13:36&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 13:37&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 13:38&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:38&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 13:40&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:40&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 13:47&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:47&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:51&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 13:51&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 13:52&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:56&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 13:56&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:57&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 13:59&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:02&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:03&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:08&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 14:08&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:09&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:11&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 14:19&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 14:19&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:20&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:21&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:22&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:23&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:24&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 14:25&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:28&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:28&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>10 14:30&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:30&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>10 14:31&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t>10 14:34&gt;&gt;&gt; 0FD8ABF6C0   None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:36&gt;&gt;&gt; 0FD8ABF6C0    </t>
+  </si>
+  <si>
+    <t>10 14:36&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 14:38&gt;&gt;&gt; 0FD8ABF6C0    </t>
+  </si>
+  <si>
+    <t>10 14:39&gt;&gt;&gt; 0FD8ABF6C0   Evony Morel</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
   <si>
     <t>August 2016</t>
-  </si>
-  <si>
-    <t>saeccffrgeaa Gary Tsai 2016-08-26 16:50:26.807392</t>
-  </si>
-  <si>
-    <t>saeccffrgea  2016-08-26 16:52:18.777307</t>
-  </si>
-  <si>
-    <t>Month</t>
   </si>
 </sst>
 </file>
@@ -89,20 +260,20 @@
     </border>
   </borders>
   <cellStyleXfs count="19">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -114,25 +285,25 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="0"/>
-    <cellStyle name="Normal 16" xfId="1"/>
-    <cellStyle name="Normal 11" xfId="2"/>
-    <cellStyle name="Normal 12" xfId="3"/>
-    <cellStyle name="Normal 17" xfId="4"/>
+    <cellStyle name="Normal 12" xfId="0"/>
+    <cellStyle name="Normal 11" xfId="1"/>
+    <cellStyle name="Normal 7" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Normal 5" xfId="4"/>
     <cellStyle builtinId="0" name="Normal" xfId="5"/>
-    <cellStyle name="Normal 7" xfId="6"/>
-    <cellStyle name="Normal 8" xfId="7"/>
-    <cellStyle name="Normal 13" xfId="8"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="9"/>
-    <cellStyle name="Normal 5" xfId="10"/>
-    <cellStyle name="Normal 14" xfId="11"/>
-    <cellStyle name="Normal 6" xfId="12"/>
-    <cellStyle name="Normal 4" xfId="13"/>
-    <cellStyle name="Normal 3" xfId="14"/>
-    <cellStyle name="Normal 9" xfId="15"/>
-    <cellStyle name="Normal 2" xfId="16"/>
-    <cellStyle name="Normal 15" xfId="17"/>
-    <cellStyle name="Normal 10" xfId="18"/>
+    <cellStyle name="Normal 9" xfId="6"/>
+    <cellStyle name="Normal 10" xfId="7"/>
+    <cellStyle name="Normal 6" xfId="8"/>
+    <cellStyle name="Normal 3" xfId="9"/>
+    <cellStyle name="Normal 2" xfId="10"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="11"/>
+    <cellStyle name="Normal 8" xfId="12"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="13"/>
+    <cellStyle name="Normal 16" xfId="14"/>
+    <cellStyle name="Normal 15" xfId="15"/>
+    <cellStyle name="Normal 17" xfId="16"/>
+    <cellStyle name="Normal 13" xfId="17"/>
+    <cellStyle name="Normal 14" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -465,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -490,6 +661,336 @@
     <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -517,12 +1018,12 @@
   <sheetData>
     <row customHeight="1" ht="19" r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
phase 1 of work study built
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132">
   <si>
     <t>January 2017</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>19 19:00&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>19 19:02&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
     <t>Month</t>
@@ -475,7 +478,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -483,6 +485,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -495,25 +498,25 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle name="Normal 9" xfId="1"/>
-    <cellStyle name="Normal 5" xfId="2"/>
-    <cellStyle name="Normal 15" xfId="3"/>
-    <cellStyle name="Normal 7" xfId="4"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
-    <cellStyle name="Normal 11" xfId="6"/>
-    <cellStyle name="Normal 3" xfId="7"/>
-    <cellStyle name="Normal 14" xfId="8"/>
-    <cellStyle name="Normal 10" xfId="9"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="10"/>
-    <cellStyle name="Normal 16" xfId="11"/>
-    <cellStyle name="Normal 2" xfId="12"/>
-    <cellStyle name="Normal 12" xfId="13"/>
-    <cellStyle name="Normal 13" xfId="14"/>
-    <cellStyle name="Normal 6" xfId="15"/>
-    <cellStyle name="Normal 8" xfId="16"/>
-    <cellStyle name="Normal 4" xfId="17"/>
-    <cellStyle name="Normal 17" xfId="18"/>
+    <cellStyle name="Normal 5" xfId="0"/>
+    <cellStyle name="Normal 11" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 9" xfId="3"/>
+    <cellStyle name="Normal 14" xfId="4"/>
+    <cellStyle name="Normal 7" xfId="5"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="6"/>
+    <cellStyle name="Normal 15" xfId="7"/>
+    <cellStyle name="Normal 13" xfId="8"/>
+    <cellStyle name="Normal 2" xfId="9"/>
+    <cellStyle name="Normal 6" xfId="10"/>
+    <cellStyle name="Normal 10" xfId="11"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="12"/>
+    <cellStyle builtinId="0" name="Normal" xfId="13"/>
+    <cellStyle name="Normal 8" xfId="14"/>
+    <cellStyle name="Normal 16" xfId="15"/>
+    <cellStyle name="Normal 12" xfId="16"/>
+    <cellStyle name="Normal 17" xfId="17"/>
+    <cellStyle name="Normal 3" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -846,7 +849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A159"/>
+  <dimension ref="A1:A160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1651,6 +1654,11 @@
     <row r="159" spans="1:1">
       <c r="A159" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1678,12 +1686,12 @@
   <sheetData>
     <row customHeight="1" ht="19" r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update reports in excel
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="208">
   <si>
     <t>January 2017</t>
   </si>
@@ -450,6 +450,189 @@
   </si>
   <si>
     <t>24 15:00&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>24 19:11&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>24 19:11&gt;&gt;&gt; 0FD88F2580   Carolyn Alana</t>
+  </si>
+  <si>
+    <t>30 16:43&gt;&gt;&gt; 4FD8A85BA0   hojin euam</t>
+  </si>
+  <si>
+    <t>30 16:43&gt;&gt;&gt; CFD8AF34C0   Megan Eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 16:47&gt;&gt;&gt; 0FD8B42CC0   </t>
+  </si>
+  <si>
+    <t>30 16:52&gt;&gt;&gt; 0FD8A290A0   Paul Fabro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 17:17&gt;&gt;&gt; 8FD89F60C0    </t>
+  </si>
+  <si>
+    <t>30 17:32&gt;&gt;&gt; 0FD8AE0B20   Anthony Rivera</t>
+  </si>
+  <si>
+    <t>30 17:39&gt;&gt;&gt; 0FD8AF13C0   Rondell Holland</t>
+  </si>
+  <si>
+    <t>30 17:39&gt;&gt;&gt; 0FD8A6BA00   John Orellana</t>
+  </si>
+  <si>
+    <t>30 17:39&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 17:39&gt;&gt;&gt; CFD8AFA4C0    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 17:40&gt;&gt;&gt; 8FD8A3A820   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 17:40&gt;&gt;&gt; CFD8AFA4C0    </t>
+  </si>
+  <si>
+    <t>30 17:40&gt;&gt;&gt; CFD8AFA4C0   arango juan</t>
+  </si>
+  <si>
+    <t>30 17:40&gt;&gt;&gt; CFD8A6B7E0   peter sormilic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 17:41&gt;&gt;&gt; 8FD8A3A820    </t>
+  </si>
+  <si>
+    <t>30 17:41&gt;&gt;&gt; 8FD8A3A820   cowell,truman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 17:41&gt;&gt;&gt; 0FD8B42CC0    </t>
+  </si>
+  <si>
+    <t>30 17:41&gt;&gt;&gt; 0FD8B42CC0   amin shahid</t>
+  </si>
+  <si>
+    <t>30 17:52&gt;&gt;&gt; 8FD8AC5D40   Rudelina Calcano</t>
+  </si>
+  <si>
+    <t>30 17:53&gt;&gt;&gt; CFD8A948E0   Vanessa Cordero</t>
+  </si>
+  <si>
+    <t>30 17:53&gt;&gt;&gt; 8FD8AC5D40   Rudelina Calcano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 17:57&gt;&gt;&gt; 8FD8B367A0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 18:01&gt;&gt;&gt; 4FD8B36A40   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 18:01&gt;&gt;&gt; 4FD8B36A40    </t>
+  </si>
+  <si>
+    <t>30 18:31&gt;&gt;&gt; 0FD88F2580   Carolyn Alana</t>
+  </si>
+  <si>
+    <t>30 19:20&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
+  </si>
+  <si>
+    <t>30 19:21&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 19:54&gt;&gt;&gt; 0FD8B45C20   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 08:27&gt;&gt;&gt; 8FD8B68DE0   </t>
+  </si>
+  <si>
+    <t>31 08:27&gt;&gt;&gt; 0FD8A6BA00   John Orellana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 08:27&gt;&gt;&gt; 8FD8B68DE0    </t>
+  </si>
+  <si>
+    <t>31 08:28&gt;&gt;&gt; 8FD8B68DE0   Miguel Martillo</t>
+  </si>
+  <si>
+    <t>31 08:52&gt;&gt;&gt; CFD88517C0   Joseph Giordano</t>
+  </si>
+  <si>
+    <t>31 09:01&gt;&gt;&gt; 0FD8A61420   Duban hershely</t>
+  </si>
+  <si>
+    <t>31 09:01&gt;&gt;&gt; CFD8A3DFA0   eugene marmontov</t>
+  </si>
+  <si>
+    <t>31 09:20&gt;&gt;&gt; 0FD8AFCD00   Joshua Itteera</t>
+  </si>
+  <si>
+    <t>31 09:21&gt;&gt;&gt; 0FD8AFCD00   Joshua Itteera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 09:26&gt;&gt;&gt; 0FD8B60440    </t>
+  </si>
+  <si>
+    <t>31 09:54&gt;&gt;&gt; 0FD89CD000   David Schachner</t>
+  </si>
+  <si>
+    <t>31 10:00&gt;&gt;&gt; CFD8ADF120   Patrick Mclaughlin</t>
+  </si>
+  <si>
+    <t>31 10:20&gt;&gt;&gt; 0FD8AD9C60   everton mendozaholmes</t>
+  </si>
+  <si>
+    <t>31 10:34&gt;&gt;&gt; 8FD87CA8C0   Dwayne Stallworth</t>
+  </si>
+  <si>
+    <t>31 10:41&gt;&gt;&gt; 4FD8AE2B20   Brandon haden</t>
+  </si>
+  <si>
+    <t>31 10:51&gt;&gt;&gt; 8FD8A60A60   ferguson elaina</t>
+  </si>
+  <si>
+    <t>31 10:53&gt;&gt;&gt; 0FD8AE0B20   Anthony Rivera</t>
+  </si>
+  <si>
+    <t>31 11:45&gt;&gt;&gt; 4FD8A51080   Calvin Y Au</t>
+  </si>
+  <si>
+    <t>31 12:02&gt;&gt;&gt; 4FD8B5DC60   Nadine Espinosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 13:15&gt;&gt;&gt; 8FD8B65040   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 13:27&gt;&gt;&gt; 0FD8B60440    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 13:37&gt;&gt;&gt; CFD8AEC840   </t>
+  </si>
+  <si>
+    <t>31 13:38&gt;&gt;&gt; 4FD8A33DE0   Anne Crosby</t>
+  </si>
+  <si>
+    <t>31 13:43&gt;&gt;&gt; 0FD8A9BD80   Jaspreet Kaur</t>
+  </si>
+  <si>
+    <t>31 13:45&gt;&gt;&gt; CFD8A948E0   Vanessa Cordero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 13:48&gt;&gt;&gt; 8FD8ADBD20   </t>
+  </si>
+  <si>
+    <t>31 13:56&gt;&gt;&gt; 0FD8AF13C0   Rondell Holland</t>
+  </si>
+  <si>
+    <t>31 14:07&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
+    <t>31 14:08&gt;&gt;&gt; 8FD8A91340   Jesse Silkworth</t>
+  </si>
+  <si>
+    <t>31 14:18&gt;&gt;&gt; CFD88517C0   Joseph Giordano</t>
+  </si>
+  <si>
+    <t>31 14:20&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
   </si>
   <si>
     <t>Month</t>
@@ -543,25 +726,25 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Normal 12" xfId="0"/>
+    <cellStyle name="Normal 8" xfId="0"/>
     <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 5" xfId="3"/>
-    <cellStyle name="Normal 6" xfId="4"/>
-    <cellStyle name="Normal 11" xfId="5"/>
-    <cellStyle name="Normal 17" xfId="6"/>
-    <cellStyle name="Normal 8" xfId="7"/>
-    <cellStyle name="Normal 10" xfId="8"/>
+    <cellStyle name="Normal 16" xfId="2"/>
+    <cellStyle name="Normal 9" xfId="3"/>
+    <cellStyle name="Normal 10" xfId="4"/>
+    <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 5" xfId="6"/>
+    <cellStyle name="Normal 13" xfId="7"/>
+    <cellStyle name="Normal 11" xfId="8"/>
     <cellStyle name="Normal 14" xfId="9"/>
     <cellStyle builtinId="0" name="Normal" xfId="10"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="11"/>
-    <cellStyle name="Normal 4" xfId="12"/>
-    <cellStyle name="Normal 13" xfId="13"/>
-    <cellStyle name="Normal 15" xfId="14"/>
-    <cellStyle name="Normal 3" xfId="15"/>
-    <cellStyle name="Normal 7" xfId="16"/>
-    <cellStyle name="Normal 16" xfId="17"/>
-    <cellStyle name="Normal 9" xfId="18"/>
+    <cellStyle name="Normal 3" xfId="11"/>
+    <cellStyle name="Normal 2" xfId="12"/>
+    <cellStyle name="Normal 7" xfId="13"/>
+    <cellStyle name="Normal 17" xfId="14"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="15"/>
+    <cellStyle name="Normal 6" xfId="16"/>
+    <cellStyle name="Normal 12" xfId="17"/>
+    <cellStyle name="Normal 15" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -894,7 +1077,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A176"/>
+  <dimension ref="A1:A241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1784,6 +1967,331 @@
     <row r="176" spans="1:1">
       <c r="A176" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1811,12 +2319,12 @@
   <sheetData>
     <row customHeight="1" ht="19" r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed and updated reporting
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="276">
   <si>
     <t>January 2017</t>
   </si>
@@ -227,7 +227,13 @@
     <t xml:space="preserve">10 13:57&gt;&gt;&gt; 0FD8ABF6C0   </t>
   </si>
   <si>
+    <t>01 19:10&gt;&gt;&gt; 0FD89CD000   David Schachner</t>
+  </si>
+  <si>
     <t xml:space="preserve">10 13:59&gt;&gt;&gt; 0FD8ABF6C0   </t>
+  </si>
+  <si>
+    <t>01 19:15&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
     <t xml:space="preserve">10 14:02&gt;&gt;&gt; 0FD8ABF6C0   </t>
@@ -892,8 +898,8 @@
   </borders>
   <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
@@ -908,10 +914,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="5" name="Percent" xfId="0"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="4" name="Currency" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
     <cellStyle builtinId="3" name="Comma" xfId="4"/>
     <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
   </cellStyles>
@@ -1555,1195 +1561,1201 @@
       <c r="A42" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="43" s="2" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="44" s="2" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="45" s="2" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="46" s="2" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="47" s="2" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="48" s="2" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="49" s="2" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="50" s="2" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="51" s="2" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="52" s="2" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="53" s="2" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="54" s="2" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="55" s="2" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="56" s="2" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="57" s="2" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="58" s="2" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="59" s="2" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="60" s="2" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="61" s="2" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="62" s="2" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="63" s="2" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="64" s="2" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="65" s="2" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="66" s="2" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="67" s="2" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="68" s="2" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="69" s="2" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="70" s="2" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="71" s="2" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="72" s="2" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="73" s="2" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="74" s="2" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="75" s="2" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="76" s="2" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="77" s="2" spans="1:2">
       <c r="A77" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="78" s="2" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="79" s="2" spans="1:2">
       <c r="A79" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="80" s="2" spans="1:2">
       <c r="A80" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="81" s="2" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="82" s="2" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="83" s="2" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="84" s="2" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="85" s="2" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="86" s="2" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="87" s="2" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="88" s="2" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="89" s="2" spans="1:2">
       <c r="A89" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="90" s="2" spans="1:2">
       <c r="A90" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="91" s="2" spans="1:2">
       <c r="A91" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="92" s="2" spans="1:2">
       <c r="A92" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="93" s="2" spans="1:2">
       <c r="A93" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="94" s="2" spans="1:2">
       <c r="A94" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="95" s="2" spans="1:2">
       <c r="A95" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="96" s="2" spans="1:2">
       <c r="A96" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="97" s="2" spans="1:2">
       <c r="A97" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="98" s="2" spans="1:2">
       <c r="A98" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="99" s="2" spans="1:2">
       <c r="A99" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="100" s="2" spans="1:2">
       <c r="A100" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="101" s="2" spans="1:2">
       <c r="A101" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="102" s="2" spans="1:2">
       <c r="A102" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="103" s="2" spans="1:2">
       <c r="A103" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="104" s="2" spans="1:2">
       <c r="A104" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="105" s="2" spans="1:2">
       <c r="A105" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="106" s="2" spans="1:2">
       <c r="A106" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="107" s="2" spans="1:2">
       <c r="A107" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="108" s="2" spans="1:2">
       <c r="A108" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="109" s="2" spans="1:2">
       <c r="A109" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="110" s="2" spans="1:2">
       <c r="A110" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="111" s="2" spans="1:2">
       <c r="A111" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="112" s="2" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="113" s="2" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="114" s="2" spans="1:2">
       <c r="A114" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="115" s="2" spans="1:2">
       <c r="A115" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="116" s="2" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="117" s="2" spans="1:2">
       <c r="A117" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="118" s="2" spans="1:2">
       <c r="A118" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="119" s="2" spans="1:2">
       <c r="A119" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="120" s="2" spans="1:2">
       <c r="A120" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="121" s="2" spans="1:2">
       <c r="A121" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="122" s="2" spans="1:2">
       <c r="A122" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="123" s="2" spans="1:2">
       <c r="A123" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="124" s="2" spans="1:2">
       <c r="A124" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="125" s="2" spans="1:2">
       <c r="A125" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="126" s="2" spans="1:2">
       <c r="A126" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="127" s="2" spans="1:2">
       <c r="A127" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="128" s="2" spans="1:2">
       <c r="A128" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="129" s="2" spans="1:2">
       <c r="A129" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="130" s="2" spans="1:2">
       <c r="A130" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="131" s="2" spans="1:2">
       <c r="A131" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="132" s="2" spans="1:2">
       <c r="A132" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="133" s="2" spans="1:2">
       <c r="A133" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="134" s="2" spans="1:2">
       <c r="A134" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="135" s="2" spans="1:2">
       <c r="A135" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="136" s="2" spans="1:2">
       <c r="A136" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="137" s="2" spans="1:2">
       <c r="A137" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="138" s="2" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="139" s="2" spans="1:2">
       <c r="A139" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="140" s="2" spans="1:2">
       <c r="A140" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="141" s="2" spans="1:2">
       <c r="A141" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="142" s="2" spans="1:2">
       <c r="A142" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="143" s="2" spans="1:2">
       <c r="A143" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="144" s="2" spans="1:2">
       <c r="A144" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="145" s="2" spans="1:2">
       <c r="A145" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="146" s="2" spans="1:2">
       <c r="A146" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="147" s="2" spans="1:2">
       <c r="A147" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="148" s="2" spans="1:2">
       <c r="A148" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="149" s="2" spans="1:2">
       <c r="A149" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="150" s="2" spans="1:2">
       <c r="A150" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="151" s="2" spans="1:2">
       <c r="A151" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="152" s="2" spans="1:2">
       <c r="A152" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="153" s="2" spans="1:2">
       <c r="A153" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="154" s="2" spans="1:2">
       <c r="A154" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="155" s="2" spans="1:2">
       <c r="A155" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="156" s="2" spans="1:2">
       <c r="A156" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="157" s="2" spans="1:2">
       <c r="A157" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="158" s="2" spans="1:2">
       <c r="A158" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="159" s="2" spans="1:2">
       <c r="A159" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="160" s="2" spans="1:2">
       <c r="A160" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="161" s="2" spans="1:2">
       <c r="A161" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="162" s="2" spans="1:2">
       <c r="A162" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="163" s="2" spans="1:2">
       <c r="A163" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="164" s="2" spans="1:2">
       <c r="A164" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="165" s="2" spans="1:2">
       <c r="A165" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="166" s="2" spans="1:2">
       <c r="A166" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="167" s="2" spans="1:2">
       <c r="A167" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="168" s="2" spans="1:2">
       <c r="A168" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="169" s="2" spans="1:2">
       <c r="A169" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="170" s="2" spans="1:2">
       <c r="A170" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="171" s="2" spans="1:2">
       <c r="A171" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="172" s="2" spans="1:2">
       <c r="A172" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="173" s="2" spans="1:2">
       <c r="A173" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="174" s="2" spans="1:2">
       <c r="A174" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="175" s="2" spans="1:2">
       <c r="A175" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="176" s="2" spans="1:2">
       <c r="A176" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="177" s="2" spans="1:2">
       <c r="A177" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="178" s="2" spans="1:2">
       <c r="A178" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="179" s="2" spans="1:2">
       <c r="A179" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="180" s="2" spans="1:2">
       <c r="A180" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="181" s="2" spans="1:2">
       <c r="A181" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="182" s="2" spans="1:2">
       <c r="A182" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="183" s="2" spans="1:2">
       <c r="A183" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="184" s="2" spans="1:2">
       <c r="A184" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="185" s="2" spans="1:2">
       <c r="A185" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="186" s="2" spans="1:2">
       <c r="A186" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="187" s="2" spans="1:2">
       <c r="A187" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="188" s="2" spans="1:2">
       <c r="A188" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="189" s="2" spans="1:2">
       <c r="A189" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="190" s="2" spans="1:2">
       <c r="A190" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="191" s="2" spans="1:2">
       <c r="A191" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="192" s="2" spans="1:2">
       <c r="A192" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="193" s="2" spans="1:2">
       <c r="A193" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="194" s="2" spans="1:2">
       <c r="A194" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="195" s="2" spans="1:2">
       <c r="A195" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="196" s="2" spans="1:2">
       <c r="A196" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="197" s="2" spans="1:2">
       <c r="A197" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="198" s="2" spans="1:2">
       <c r="A198" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="199" s="2" spans="1:2">
       <c r="A199" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="200" s="2" spans="1:2">
       <c r="A200" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="201" s="2" spans="1:2">
       <c r="A201" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="202" s="2" spans="1:2">
       <c r="A202" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="203" s="2" spans="1:2">
       <c r="A203" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="204" s="2" spans="1:2">
       <c r="A204" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="205" s="2" spans="1:2">
       <c r="A205" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="206" s="2" spans="1:2">
       <c r="A206" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="207" s="2" spans="1:2">
       <c r="A207" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="208" s="2" spans="1:2">
       <c r="A208" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="209" s="2" spans="1:2">
       <c r="A209" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="210" s="2" spans="1:2">
       <c r="A210" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="211" s="2" spans="1:2">
       <c r="A211" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="212" s="2" spans="1:2">
       <c r="A212" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="213" s="2" spans="1:2">
       <c r="A213" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="214" s="2" spans="1:2">
       <c r="A214" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="215" s="2" spans="1:2">
       <c r="A215" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="216" s="2" spans="1:2">
       <c r="A216" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="217" s="2" spans="1:2">
       <c r="A217" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="218" s="2" spans="1:2">
       <c r="A218" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="219" s="2" spans="1:2">
       <c r="A219" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="220" s="2" spans="1:2">
       <c r="A220" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="221" s="2" spans="1:2">
       <c r="A221" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="222" s="2" spans="1:2">
       <c r="A222" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="223" s="2" spans="1:2">
       <c r="A223" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="224" s="2" spans="1:2">
       <c r="A224" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="225" s="2" spans="1:2">
       <c r="A225" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="226" s="2" spans="1:2">
       <c r="A226" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="227" s="2" spans="1:2">
       <c r="A227" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="228" s="2" spans="1:2">
       <c r="A228" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="229" s="2" spans="1:2">
       <c r="A229" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="230" s="2" spans="1:2">
       <c r="A230" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="231" s="2" spans="1:2">
       <c r="A231" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="232" s="2" spans="1:2">
       <c r="A232" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="233" s="2" spans="1:2">
       <c r="A233" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="234" s="2" spans="1:2">
       <c r="A234" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="235" s="2" spans="1:2">
       <c r="A235" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="236" s="2" spans="1:2">
       <c r="A236" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="237" s="2" spans="1:2">
       <c r="A237" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="238" s="2" spans="1:2">
       <c r="A238" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="239" s="2" spans="1:2">
       <c r="A239" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="240" s="2" spans="1:2">
       <c r="A240" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="241" s="2" spans="1:2">
       <c r="A241" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="242" s="2" spans="1:2">
       <c r="A242" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="243" s="2" spans="1:2">
       <c r="A243" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="244" s="2" spans="1:2">
       <c r="A244" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="245" s="2" spans="1:2">
       <c r="A245" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="246" s="2" spans="1:2">
       <c r="A246" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="247" s="2" spans="1:2">
       <c r="A247" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="248" s="2" spans="1:2">
       <c r="A248" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="249" s="2" spans="1:2">
       <c r="A249" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="250" s="2" spans="1:2">
       <c r="A250" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="251" s="2" spans="1:2">
       <c r="A251" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="252" s="2" spans="1:2">
       <c r="A252" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="253" s="2" spans="1:2">
       <c r="A253" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="254" s="2" spans="1:2">
       <c r="A254" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="255" s="2" spans="1:2">
       <c r="A255" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="256" s="2" spans="1:2">
       <c r="A256" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="257" s="2" spans="1:2">
       <c r="A257" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="258" s="2" spans="1:2">
       <c r="A258" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="259" s="2" spans="1:2">
       <c r="A259" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="260" s="2" spans="1:2">
       <c r="A260" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="261" s="2" spans="1:2">
       <c r="A261" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="262" s="2" spans="1:2">
       <c r="A262" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="263" s="2" spans="1:2">
       <c r="A263" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="264" s="2" spans="1:2">
       <c r="A264" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="265" s="2" spans="1:2">
       <c r="A265" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="266" s="2" spans="1:2">
       <c r="A266" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="267" s="2" spans="1:2">
       <c r="A267" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="268" s="2" spans="1:2">
       <c r="A268" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="269" s="2" spans="1:2">
       <c r="A269" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="270" s="2" spans="1:2">
       <c r="A270" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="271" s="2" spans="1:2">
       <c r="A271" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="272" s="2" spans="1:2">
       <c r="A272" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="273" s="2" spans="1:2">
       <c r="A273" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="274" s="2" spans="1:2">
       <c r="A274" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="275" s="2" spans="1:2">
       <c r="A275" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="276" s="2" spans="1:2">
       <c r="A276" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="277" s="2" spans="1:2">
       <c r="A277" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="278" s="2" spans="1:2">
       <c r="A278" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="279" s="2" spans="1:2">
       <c r="A279" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="280" s="2" spans="1:2">
       <c r="A280" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2773,12 +2785,12 @@
   <sheetData>
     <row customHeight="1" ht="19" r="1" s="2" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="2" s="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work study is operational
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="463">
   <si>
     <t>January 2017</t>
   </si>
@@ -866,211 +866,433 @@
     <t>20 14:58&gt;&gt;&gt; 0FD89CD000   David Schachner</t>
   </si>
   <si>
+    <t>07 12:19&gt;&gt;&gt; 0FD8A6BA00   John Orellana</t>
+  </si>
+  <si>
     <t>23 08:55&gt;&gt;&gt; 0FD8AE8B60   Natalie Primus</t>
   </si>
   <si>
+    <t>07 12:21&gt;&gt;&gt; CFD89A9C80   Bryan Williams</t>
+  </si>
+  <si>
     <t>23 09:10&gt;&gt;&gt; 0FD89CD000   David Schachner</t>
   </si>
   <si>
+    <t>07 12:21&gt;&gt;&gt; 0FD8AF9E00   Karla Pimentel</t>
+  </si>
+  <si>
     <t>23 11:03&gt;&gt;&gt; CFD88517C0   Joseph Giordano</t>
   </si>
   <si>
     <t>24 12:58&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
+    <t>07 12:43&gt;&gt;&gt; 0FD8B4E900   Carlos De Los Santos</t>
+  </si>
+  <si>
     <t>24 14:26&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
+    <t>07 13:07&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
+  </si>
+  <si>
     <t>24 14:28&gt;&gt;&gt; 8FD8A5E5E0   Anthony Avevor</t>
   </si>
   <si>
+    <t>07 13:10&gt;&gt;&gt; 4FD8A85BA0   hojin euam</t>
+  </si>
+  <si>
     <t>24 14:37&gt;&gt;&gt; 8FD8A5E5E0   Anthony Avevor</t>
   </si>
   <si>
+    <t xml:space="preserve">07 13:11&gt;&gt;&gt; 8FD8985540    </t>
+  </si>
+  <si>
     <t>24 14:39&gt;&gt;&gt; 8FD8A5E5E0   Anthony Avevor</t>
   </si>
   <si>
+    <t xml:space="preserve">07 13:32&gt;&gt;&gt; 8FD8A8D440    </t>
+  </si>
+  <si>
     <t>24 14:39&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
+    <t>07 13:34&gt;&gt;&gt; 8FD8ADBD20   david orlando</t>
+  </si>
+  <si>
     <t>24 14:48&gt;&gt;&gt; CFD8A948E0   Vanessa Cordero</t>
   </si>
   <si>
+    <t xml:space="preserve">07 13:42&gt;&gt;&gt; 8FD8B39BA0   </t>
+  </si>
+  <si>
     <t>24 14:56&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
+    <t>07 13:53&gt;&gt;&gt; 8FD8A91340   Jesse Silkworth</t>
+  </si>
+  <si>
+    <t>07 14:07&gt;&gt;&gt; CFD8A948E0   Vanessa Cordero</t>
+  </si>
+  <si>
     <t>24 14:57&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
+    <t>07 15:28&gt;&gt;&gt; 8FD8AFD100   rahyner penaranda</t>
+  </si>
+  <si>
     <t>24 15:00&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
+    <t>07 15:40&gt;&gt;&gt; 0FD8A6BA00   John Orellana</t>
+  </si>
+  <si>
     <t>24 19:11&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
   </si>
   <si>
+    <t>07 15:48&gt;&gt;&gt; 0FD8AD42A0   Covalky Pena</t>
+  </si>
+  <si>
     <t>24 19:11&gt;&gt;&gt; 0FD88F2580   Carolyn Alana</t>
   </si>
   <si>
+    <t>07 16:12&gt;&gt;&gt; 0FD8A9BD80   Jaspreet Kaur</t>
+  </si>
+  <si>
     <t>30 16:43&gt;&gt;&gt; 4FD8A85BA0   hojin euam</t>
   </si>
   <si>
+    <t>07 16:23&gt;&gt;&gt; CFD8A3DFA0   eugene marmontov</t>
+  </si>
+  <si>
+    <t>07 17:19&gt;&gt;&gt; 0FD88F2580   Carolyn Alana</t>
+  </si>
+  <si>
     <t>30 16:43&gt;&gt;&gt; CFD8AF34C0   Megan Eng</t>
   </si>
   <si>
+    <t>07 17:47&gt;&gt;&gt; 4FD87F2960   Thomas Yoo</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 16:47&gt;&gt;&gt; 0FD8B42CC0   </t>
   </si>
   <si>
+    <t>07 17:48&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
     <t>30 16:52&gt;&gt;&gt; 0FD8A290A0   Paul Fabro</t>
   </si>
   <si>
+    <t>07 19:10&gt;&gt;&gt; 0FD8AD42A0   Covalky Pena</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 17:17&gt;&gt;&gt; 8FD89F60C0    </t>
   </si>
   <si>
+    <t>07 19:10&gt;&gt;&gt; 0FD8B5ED00   Crosby anne</t>
+  </si>
+  <si>
     <t>30 17:32&gt;&gt;&gt; 0FD8AE0B20   Anthony Rivera</t>
   </si>
   <si>
+    <t>07 19:55&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
     <t>30 17:39&gt;&gt;&gt; 0FD8AF13C0   Rondell Holland</t>
   </si>
   <si>
+    <t>08 08:53&gt;&gt;&gt; 4FD8A33DE0   Anne Crosby</t>
+  </si>
+  <si>
     <t>30 17:39&gt;&gt;&gt; 0FD8A6BA00   John Orellana</t>
   </si>
   <si>
+    <t>08 08:54&gt;&gt;&gt; 0FD8AE8B60   Natalie Primus</t>
+  </si>
+  <si>
     <t>30 17:39&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
   </si>
   <si>
+    <t>08 09:07&gt;&gt;&gt; 8FD8AEB240   luciano.ibbott</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 17:39&gt;&gt;&gt; CFD8AFA4C0    </t>
   </si>
   <si>
+    <t>08 09:14&gt;&gt;&gt; 8FD8B68DE0   Miguel Martillo</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 17:40&gt;&gt;&gt; 8FD8A3A820   </t>
   </si>
   <si>
+    <t>08 09:42&gt;&gt;&gt; 4FD8A51080   Calvin Y Au</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 17:40&gt;&gt;&gt; CFD8AFA4C0    </t>
   </si>
   <si>
+    <t>08 09:52&gt;&gt;&gt; 8FD8AC1E00   Kimberly Pierre</t>
+  </si>
+  <si>
     <t>30 17:40&gt;&gt;&gt; CFD8AFA4C0   arango juan</t>
   </si>
   <si>
+    <t>08 09:54&gt;&gt;&gt; 4FD8B41A40   Justin Davis</t>
+  </si>
+  <si>
     <t>30 17:40&gt;&gt;&gt; CFD8A6B7E0   peter sormilic</t>
   </si>
   <si>
+    <t>08 10:03&gt;&gt;&gt; 0FD89CD000   David Schachner</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 17:41&gt;&gt;&gt; 8FD8A3A820    </t>
   </si>
   <si>
+    <t xml:space="preserve">08 10:04&gt;&gt;&gt; CFD8B45C40   </t>
+  </si>
+  <si>
     <t>30 17:41&gt;&gt;&gt; 8FD8A3A820   cowell,truman</t>
   </si>
   <si>
+    <t>08 10:04&gt;&gt;&gt; CFD8A6B7E0   peter sormilic</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 17:41&gt;&gt;&gt; 0FD8B42CC0    </t>
   </si>
   <si>
+    <t>08 10:28&gt;&gt;&gt; 0FD8B5ED00   Crosby anne</t>
+  </si>
+  <si>
     <t>30 17:41&gt;&gt;&gt; 0FD8B42CC0   amin shahid</t>
   </si>
   <si>
+    <t>08 10:30&gt;&gt;&gt; 0FD8A83600   douglas smith</t>
+  </si>
+  <si>
     <t>30 17:52&gt;&gt;&gt; 8FD8AC5D40   Rudelina Calcano</t>
   </si>
   <si>
+    <t xml:space="preserve">08 10:37&gt;&gt;&gt; 8FD88BA9C0    </t>
+  </si>
+  <si>
     <t>30 17:53&gt;&gt;&gt; CFD8A948E0   Vanessa Cordero</t>
   </si>
   <si>
+    <t>08 11:11&gt;&gt;&gt; 0FD899D9C0   cammy-el allen</t>
+  </si>
+  <si>
+    <t>08 11:26&gt;&gt;&gt; 0FD8ACF700   Jared Amuso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 11:30&gt;&gt;&gt; 0FD89E2980   </t>
+  </si>
+  <si>
     <t>30 17:53&gt;&gt;&gt; 8FD8AC5D40   Rudelina Calcano</t>
   </si>
   <si>
+    <t xml:space="preserve">08 11:41&gt;&gt;&gt; 8FD8AEA680   </t>
+  </si>
+  <si>
     <t xml:space="preserve">30 17:57&gt;&gt;&gt; 8FD8B367A0   </t>
   </si>
   <si>
+    <t>08 11:58&gt;&gt;&gt; 4FD8A33DE0   Anne Crosby</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 18:01&gt;&gt;&gt; 4FD8B36A40   </t>
   </si>
   <si>
+    <t>08 12:21&gt;&gt;&gt; 4FD87D1F40   Gao Feng</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 18:01&gt;&gt;&gt; 4FD8B36A40    </t>
   </si>
   <si>
+    <t>08 12:22&gt;&gt;&gt; 0FD88F2580   Carolyn Alana</t>
+  </si>
+  <si>
     <t>30 18:31&gt;&gt;&gt; 0FD88F2580   Carolyn Alana</t>
   </si>
   <si>
+    <t xml:space="preserve">08 12:49&gt;&gt;&gt; CFD8B3CA60   </t>
+  </si>
+  <si>
     <t>30 19:20&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
   </si>
   <si>
+    <t>08 12:49&gt;&gt;&gt; 4FD8AB6C20   Freddy Beltran</t>
+  </si>
+  <si>
     <t>30 19:21&gt;&gt;&gt; 0FD8AFD720   Jennifer Mercedes</t>
   </si>
   <si>
+    <t xml:space="preserve">08 13:09&gt;&gt;&gt; 0FD8AE84A0    </t>
+  </si>
+  <si>
     <t xml:space="preserve">30 19:54&gt;&gt;&gt; 0FD8B45C20   </t>
   </si>
   <si>
+    <t xml:space="preserve">08 13:18&gt;&gt;&gt; CFD8B6A840   </t>
+  </si>
+  <si>
     <t xml:space="preserve">31 08:27&gt;&gt;&gt; 8FD8B68DE0   </t>
   </si>
   <si>
+    <t xml:space="preserve">08 13:23&gt;&gt;&gt; 4FD8B3E300   </t>
+  </si>
+  <si>
     <t>31 08:27&gt;&gt;&gt; 0FD8A6BA00   John Orellana</t>
   </si>
   <si>
+    <t>08 13:25&gt;&gt;&gt; 8FD8AFF180   Oscar Chicaiza</t>
+  </si>
+  <si>
     <t xml:space="preserve">31 08:27&gt;&gt;&gt; 8FD8B68DE0    </t>
   </si>
   <si>
+    <t>08 13:25&gt;&gt;&gt; 4FD8B41A40   Justin Davis</t>
+  </si>
+  <si>
     <t>31 08:28&gt;&gt;&gt; 8FD8B68DE0   Miguel Martillo</t>
   </si>
   <si>
+    <t>08 13:27&gt;&gt;&gt; 8FD8A5D640   Anwar Sufian</t>
+  </si>
+  <si>
     <t>31 08:52&gt;&gt;&gt; CFD88517C0   Joseph Giordano</t>
   </si>
   <si>
+    <t>08 13:33&gt;&gt;&gt; 8FD8A3A820   cowell,truman</t>
+  </si>
+  <si>
     <t>31 09:01&gt;&gt;&gt; 0FD8A61420   Duban hershely</t>
   </si>
   <si>
+    <t>08 13:35&gt;&gt;&gt; 8FD87CA8C0   Dwayne Stallworth</t>
+  </si>
+  <si>
     <t>31 09:01&gt;&gt;&gt; CFD8A3DFA0   eugene marmontov</t>
   </si>
   <si>
+    <t xml:space="preserve">08 13:36&gt;&gt;&gt; 8FD8B367A0    </t>
+  </si>
+  <si>
     <t>31 09:20&gt;&gt;&gt; 0FD8AFCD00   Joshua Itteera</t>
   </si>
   <si>
+    <t>08 13:36&gt;&gt;&gt; 0FD8AE0B20   Anthony Rivera</t>
+  </si>
+  <si>
     <t>31 09:21&gt;&gt;&gt; 0FD8AFCD00   Joshua Itteera</t>
   </si>
   <si>
+    <t xml:space="preserve">08 13:38&gt;&gt;&gt; 0FD8AC1480   </t>
+  </si>
+  <si>
     <t xml:space="preserve">31 09:26&gt;&gt;&gt; 0FD8B60440    </t>
   </si>
   <si>
+    <t>08 13:39&gt;&gt;&gt; 0FD8AF13C0   Rondell Holland</t>
+  </si>
+  <si>
     <t>31 09:54&gt;&gt;&gt; 0FD89CD000   David Schachner</t>
   </si>
   <si>
+    <t>08 13:40&gt;&gt;&gt; 8FD8A57200   Averill Curameng</t>
+  </si>
+  <si>
     <t>31 10:00&gt;&gt;&gt; CFD8ADF120   Patrick Mclaughlin</t>
   </si>
   <si>
+    <t>08 15:02&gt;&gt;&gt; 0FD8B5ED00   Crosby anne</t>
+  </si>
+  <si>
     <t>31 10:20&gt;&gt;&gt; 0FD8AD9C60   everton mendozaholmes</t>
   </si>
   <si>
+    <t>08 15:44&gt;&gt;&gt; 0FD8AD42A0   Covalky Pena</t>
+  </si>
+  <si>
     <t>31 10:34&gt;&gt;&gt; 8FD87CA8C0   Dwayne Stallworth</t>
   </si>
   <si>
+    <t xml:space="preserve">08 15:45&gt;&gt;&gt; 0FD8A87380   Crystal Evelyn </t>
+  </si>
+  <si>
     <t>31 10:41&gt;&gt;&gt; 4FD8AE2B20   Brandon haden</t>
   </si>
   <si>
+    <t>08 15:50&gt;&gt;&gt; CFD8AFA4C0   arango juan</t>
+  </si>
+  <si>
     <t>31 10:51&gt;&gt;&gt; 8FD8A60A60   ferguson elaina</t>
   </si>
   <si>
+    <t>08 15:52&gt;&gt;&gt; 4FD8A85BA0   hojin euam</t>
+  </si>
+  <si>
     <t>31 10:53&gt;&gt;&gt; 0FD8AE0B20   Anthony Rivera</t>
   </si>
   <si>
+    <t>08 16:11&gt;&gt;&gt; 8FD8A5E5E0   Anthony Avevor</t>
+  </si>
+  <si>
     <t>31 11:45&gt;&gt;&gt; 4FD8A51080   Calvin Y Au</t>
   </si>
   <si>
+    <t>08 16:27&gt;&gt;&gt; 0FD89CD000   David Schachner</t>
+  </si>
+  <si>
     <t>31 12:02&gt;&gt;&gt; 4FD8B5DC60   Nadine Espinosa</t>
   </si>
   <si>
+    <t>08 17:14&gt;&gt;&gt; 8FD8A5D640   Anwar Sufian</t>
+  </si>
+  <si>
     <t xml:space="preserve">31 13:15&gt;&gt;&gt; 8FD8B65040   </t>
   </si>
   <si>
+    <t>08 18:04&gt;&gt;&gt; 0FD8B5ED00   Crosby anne</t>
+  </si>
+  <si>
     <t xml:space="preserve">31 13:27&gt;&gt;&gt; 0FD8B60440    </t>
   </si>
   <si>
+    <t>08 18:52&gt;&gt;&gt; CFD8A78940   Nicole Latta</t>
+  </si>
+  <si>
     <t xml:space="preserve">31 13:37&gt;&gt;&gt; CFD8AEC840   </t>
   </si>
   <si>
+    <t xml:space="preserve">08 19:11&gt;&gt;&gt; CFD8B45C40    </t>
+  </si>
+  <si>
     <t>31 13:38&gt;&gt;&gt; 4FD8A33DE0   Anne Crosby</t>
   </si>
   <si>
+    <t>08 20:41&gt;&gt;&gt; CFD893A460   Gary Tsai</t>
+  </si>
+  <si>
     <t>31 13:43&gt;&gt;&gt; 0FD8A9BD80   Jaspreet Kaur</t>
   </si>
   <si>
+    <t>08 20:44&gt;&gt;&gt; 4FD8A85BA0   hojin euam</t>
+  </si>
+  <si>
     <t>31 13:45&gt;&gt;&gt; CFD8A948E0   Vanessa Cordero</t>
   </si>
   <si>
+    <t>08 20:46&gt;&gt;&gt; 4FD8A85BA0   hojin euam</t>
+  </si>
+  <si>
+    <t>08 20:47&gt;&gt;&gt; 0FD8AF13C0   Rondell Holland</t>
+  </si>
+  <si>
     <t xml:space="preserve">31 13:48&gt;&gt;&gt; 8FD8ADBD20   </t>
+  </si>
+  <si>
+    <t>08 20:51&gt;&gt;&gt; 8FD894EAC0   Sade Thomas</t>
   </si>
   <si>
     <t>31 13:56&gt;&gt;&gt; 0FD8AF13C0   Rondell Holland</t>
@@ -1236,12 +1458,12 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -1253,12 +1475,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="3" name="Comma" xfId="0"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="1"/>
-    <cellStyle builtinId="4" name="Currency" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="5" name="Percent" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
     <cellStyle builtinId="7" name="Currency [0]" xfId="3"/>
-    <cellStyle builtinId="5" name="Percent" xfId="4"/>
-    <cellStyle builtinId="0" name="Normal" xfId="5"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -2860,595 +3082,823 @@
       <c r="A162" s="1" t="s">
         <v>282</v>
       </c>
+      <c r="B162" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="163" s="2" spans="1:2">
       <c r="A163" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="B163" t="s">
+        <v>285</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="164" s="2" spans="1:2">
       <c r="A164" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
+      </c>
+      <c r="B164" t="s">
+        <v>287</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="165" s="2" spans="1:2">
       <c r="A165" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
+      </c>
+      <c r="B165" t="s">
+        <v>287</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="166" s="2" spans="1:2">
       <c r="A166" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
+      </c>
+      <c r="B166" t="s">
+        <v>290</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="167" s="2" spans="1:2">
       <c r="A167" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
+      </c>
+      <c r="B167" t="s">
+        <v>292</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="168" s="2" spans="1:2">
       <c r="A168" s="1" t="s">
-        <v>288</v>
+        <v>293</v>
+      </c>
+      <c r="B168" t="s">
+        <v>294</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="169" s="2" spans="1:2">
       <c r="A169" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
+      </c>
+      <c r="B169" t="s">
+        <v>296</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="170" s="2" spans="1:2">
       <c r="A170" s="1" t="s">
-        <v>290</v>
+        <v>297</v>
+      </c>
+      <c r="B170" t="s">
+        <v>298</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="171" s="2" spans="1:2">
       <c r="A171" s="1" t="s">
-        <v>291</v>
+        <v>299</v>
+      </c>
+      <c r="B171" t="s">
+        <v>300</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="172" s="2" spans="1:2">
       <c r="A172" s="1" t="s">
-        <v>292</v>
+        <v>301</v>
+      </c>
+      <c r="B172" t="s">
+        <v>302</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="173" s="2" spans="1:2">
       <c r="A173" s="1" t="s">
-        <v>293</v>
+        <v>303</v>
+      </c>
+      <c r="B173" t="s">
+        <v>304</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="174" s="2" spans="1:2">
       <c r="A174" s="1" t="s">
-        <v>293</v>
+        <v>303</v>
+      </c>
+      <c r="B174" t="s">
+        <v>305</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="175" s="2" spans="1:2">
       <c r="A175" s="1" t="s">
-        <v>294</v>
+        <v>306</v>
+      </c>
+      <c r="B175" t="s">
+        <v>307</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="176" s="2" spans="1:2">
       <c r="A176" s="1" t="s">
-        <v>295</v>
+        <v>308</v>
+      </c>
+      <c r="B176" t="s">
+        <v>309</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="177" s="2" spans="1:2">
       <c r="A177" s="1" t="s">
-        <v>296</v>
+        <v>310</v>
+      </c>
+      <c r="B177" t="s">
+        <v>311</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="178" s="2" spans="1:2">
       <c r="A178" s="1" t="s">
-        <v>297</v>
+        <v>312</v>
+      </c>
+      <c r="B178" t="s">
+        <v>313</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="179" s="2" spans="1:2">
       <c r="A179" s="1" t="s">
-        <v>298</v>
+        <v>314</v>
+      </c>
+      <c r="B179" t="s">
+        <v>315</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="180" s="2" spans="1:2">
       <c r="A180" s="1" t="s">
-        <v>298</v>
+        <v>314</v>
+      </c>
+      <c r="B180" t="s">
+        <v>316</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="181" s="2" spans="1:2">
       <c r="A181" s="1" t="s">
-        <v>299</v>
+        <v>317</v>
+      </c>
+      <c r="B181" t="s">
+        <v>318</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="182" s="2" spans="1:2">
       <c r="A182" s="1" t="s">
-        <v>300</v>
+        <v>319</v>
+      </c>
+      <c r="B182" t="s">
+        <v>320</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="183" s="2" spans="1:2">
       <c r="A183" s="1" t="s">
-        <v>301</v>
+        <v>321</v>
+      </c>
+      <c r="B183" t="s">
+        <v>322</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="184" s="2" spans="1:2">
       <c r="A184" s="1" t="s">
-        <v>302</v>
+        <v>323</v>
+      </c>
+      <c r="B184" t="s">
+        <v>324</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="185" s="2" spans="1:2">
       <c r="A185" s="1" t="s">
-        <v>303</v>
+        <v>325</v>
+      </c>
+      <c r="B185" t="s">
+        <v>326</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="186" s="2" spans="1:2">
       <c r="A186" s="1" t="s">
-        <v>304</v>
+        <v>327</v>
+      </c>
+      <c r="B186" t="s">
+        <v>328</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="187" s="2" spans="1:2">
       <c r="A187" s="1" t="s">
-        <v>305</v>
+        <v>329</v>
+      </c>
+      <c r="B187" t="s">
+        <v>330</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="188" s="2" spans="1:2">
       <c r="A188" s="1" t="s">
-        <v>306</v>
+        <v>331</v>
+      </c>
+      <c r="B188" t="s">
+        <v>332</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="189" s="2" spans="1:2">
       <c r="A189" s="1" t="s">
-        <v>307</v>
+        <v>333</v>
+      </c>
+      <c r="B189" t="s">
+        <v>334</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="190" s="2" spans="1:2">
       <c r="A190" s="1" t="s">
-        <v>308</v>
+        <v>335</v>
+      </c>
+      <c r="B190" t="s">
+        <v>336</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="191" s="2" spans="1:2">
       <c r="A191" s="1" t="s">
-        <v>309</v>
+        <v>337</v>
+      </c>
+      <c r="B191" t="s">
+        <v>338</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="192" s="2" spans="1:2">
       <c r="A192" s="1" t="s">
-        <v>310</v>
+        <v>339</v>
+      </c>
+      <c r="B192" t="s">
+        <v>340</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="193" s="2" spans="1:2">
       <c r="A193" s="1" t="s">
-        <v>311</v>
+        <v>341</v>
+      </c>
+      <c r="B193" t="s">
+        <v>342</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="194" s="2" spans="1:2">
       <c r="A194" s="1" t="s">
-        <v>312</v>
+        <v>343</v>
+      </c>
+      <c r="B194" t="s">
+        <v>344</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="195" s="2" spans="1:2">
       <c r="A195" s="1" t="s">
-        <v>313</v>
+        <v>345</v>
+      </c>
+      <c r="B195" t="s">
+        <v>346</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="196" s="2" spans="1:2">
       <c r="A196" s="1" t="s">
-        <v>314</v>
+        <v>347</v>
+      </c>
+      <c r="B196" t="s">
+        <v>348</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="197" s="2" spans="1:2">
       <c r="A197" s="1" t="s">
-        <v>315</v>
+        <v>349</v>
+      </c>
+      <c r="B197" t="s">
+        <v>350</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="198" s="2" spans="1:2">
       <c r="A198" s="1" t="s">
-        <v>316</v>
+        <v>351</v>
+      </c>
+      <c r="B198" t="s">
+        <v>352</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="199" s="2" spans="1:2">
       <c r="A199" s="1" t="s">
-        <v>317</v>
+        <v>353</v>
+      </c>
+      <c r="B199" t="s">
+        <v>354</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="200" s="2" spans="1:2">
       <c r="A200" s="1" t="s">
-        <v>317</v>
+        <v>353</v>
+      </c>
+      <c r="B200" t="s">
+        <v>355</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="201" s="2" spans="1:2">
       <c r="A201" s="1" t="s">
-        <v>317</v>
+        <v>353</v>
+      </c>
+      <c r="B201" t="s">
+        <v>356</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="202" s="2" spans="1:2">
       <c r="A202" s="1" t="s">
-        <v>318</v>
+        <v>357</v>
+      </c>
+      <c r="B202" t="s">
+        <v>358</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="203" s="2" spans="1:2">
       <c r="A203" s="1" t="s">
-        <v>319</v>
+        <v>359</v>
+      </c>
+      <c r="B203" t="s">
+        <v>360</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="204" s="2" spans="1:2">
       <c r="A204" s="1" t="s">
-        <v>320</v>
+        <v>361</v>
+      </c>
+      <c r="B204" t="s">
+        <v>362</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="205" s="2" spans="1:2">
       <c r="A205" s="1" t="s">
-        <v>321</v>
+        <v>363</v>
+      </c>
+      <c r="B205" t="s">
+        <v>364</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="206" s="2" spans="1:2">
       <c r="A206" s="1" t="s">
-        <v>322</v>
+        <v>365</v>
+      </c>
+      <c r="B206" t="s">
+        <v>366</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="207" s="2" spans="1:2">
       <c r="A207" s="1" t="s">
-        <v>323</v>
+        <v>367</v>
+      </c>
+      <c r="B207" t="s">
+        <v>368</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="208" s="2" spans="1:2">
       <c r="A208" s="1" t="s">
-        <v>324</v>
+        <v>369</v>
+      </c>
+      <c r="B208" t="s">
+        <v>370</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="209" s="2" spans="1:2">
       <c r="A209" s="1" t="s">
-        <v>325</v>
+        <v>371</v>
+      </c>
+      <c r="B209" t="s">
+        <v>372</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="210" s="2" spans="1:2">
       <c r="A210" s="1" t="s">
-        <v>326</v>
+        <v>373</v>
+      </c>
+      <c r="B210" t="s">
+        <v>374</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="211" s="2" spans="1:2">
       <c r="A211" s="1" t="s">
-        <v>327</v>
+        <v>375</v>
+      </c>
+      <c r="B211" t="s">
+        <v>376</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="212" s="2" spans="1:2">
       <c r="A212" s="1" t="s">
-        <v>328</v>
+        <v>377</v>
+      </c>
+      <c r="B212" t="s">
+        <v>378</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="213" s="2" spans="1:2">
       <c r="A213" s="1" t="s">
-        <v>329</v>
+        <v>379</v>
+      </c>
+      <c r="B213" t="s">
+        <v>380</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="214" s="2" spans="1:2">
       <c r="A214" s="1" t="s">
-        <v>330</v>
+        <v>381</v>
+      </c>
+      <c r="B214" t="s">
+        <v>382</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="215" s="2" spans="1:2">
       <c r="A215" s="1" t="s">
-        <v>331</v>
+        <v>383</v>
+      </c>
+      <c r="B215" t="s">
+        <v>384</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="216" s="2" spans="1:2">
       <c r="A216" s="1" t="s">
-        <v>332</v>
+        <v>385</v>
+      </c>
+      <c r="B216" t="s">
+        <v>386</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="217" s="2" spans="1:2">
       <c r="A217" s="1" t="s">
-        <v>333</v>
+        <v>387</v>
+      </c>
+      <c r="B217" t="s">
+        <v>388</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="218" s="2" spans="1:2">
       <c r="A218" s="1" t="s">
-        <v>334</v>
+        <v>389</v>
+      </c>
+      <c r="B218" t="s">
+        <v>390</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="219" s="2" spans="1:2">
       <c r="A219" s="1" t="s">
-        <v>335</v>
+        <v>391</v>
+      </c>
+      <c r="B219" t="s">
+        <v>392</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="220" s="2" spans="1:2">
       <c r="A220" s="1" t="s">
-        <v>336</v>
+        <v>393</v>
+      </c>
+      <c r="B220" t="s">
+        <v>394</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="221" s="2" spans="1:2">
       <c r="A221" s="1" t="s">
-        <v>337</v>
+        <v>395</v>
+      </c>
+      <c r="B221" t="s">
+        <v>396</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="222" s="2" spans="1:2">
       <c r="A222" s="1" t="s">
-        <v>338</v>
+        <v>397</v>
+      </c>
+      <c r="B222" t="s">
+        <v>398</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="223" s="2" spans="1:2">
       <c r="A223" s="1" t="s">
-        <v>339</v>
+        <v>399</v>
+      </c>
+      <c r="B223" t="s">
+        <v>400</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="224" s="2" spans="1:2">
       <c r="A224" s="1" t="s">
-        <v>340</v>
+        <v>401</v>
+      </c>
+      <c r="B224" t="s">
+        <v>402</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="225" s="2" spans="1:2">
       <c r="A225" s="1" t="s">
-        <v>341</v>
+        <v>403</v>
+      </c>
+      <c r="B225" t="s">
+        <v>404</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="226" s="2" spans="1:2">
       <c r="A226" s="1" t="s">
-        <v>342</v>
+        <v>405</v>
+      </c>
+      <c r="B226" t="s">
+        <v>406</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="227" s="2" spans="1:2">
       <c r="A227" s="1" t="s">
-        <v>343</v>
+        <v>407</v>
+      </c>
+      <c r="B227" t="s">
+        <v>408</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="228" s="2" spans="1:2">
       <c r="A228" s="1" t="s">
-        <v>344</v>
+        <v>409</v>
+      </c>
+      <c r="B228" t="s">
+        <v>410</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="229" s="2" spans="1:2">
       <c r="A229" s="1" t="s">
-        <v>345</v>
+        <v>411</v>
+      </c>
+      <c r="B229" t="s">
+        <v>412</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="230" s="2" spans="1:2">
       <c r="A230" s="1" t="s">
-        <v>346</v>
+        <v>413</v>
+      </c>
+      <c r="B230" t="s">
+        <v>414</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="231" s="2" spans="1:2">
       <c r="A231" s="1" t="s">
-        <v>347</v>
+        <v>415</v>
+      </c>
+      <c r="B231" t="s">
+        <v>416</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="232" s="2" spans="1:2">
       <c r="A232" s="1" t="s">
-        <v>348</v>
+        <v>417</v>
+      </c>
+      <c r="B232" t="s">
+        <v>418</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="233" s="2" spans="1:2">
       <c r="A233" s="1" t="s">
-        <v>349</v>
+        <v>419</v>
+      </c>
+      <c r="B233" t="s">
+        <v>420</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="234" s="2" spans="1:2">
       <c r="A234" s="1" t="s">
-        <v>350</v>
+        <v>421</v>
+      </c>
+      <c r="B234" t="s">
+        <v>422</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="235" s="2" spans="1:2">
       <c r="A235" s="1" t="s">
-        <v>350</v>
+        <v>421</v>
+      </c>
+      <c r="B235" t="s">
+        <v>423</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="236" s="2" spans="1:2">
       <c r="A236" s="1" t="s">
-        <v>351</v>
+        <v>424</v>
+      </c>
+      <c r="B236" t="s">
+        <v>425</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="237" s="2" spans="1:2">
       <c r="A237" s="1" t="s">
-        <v>352</v>
+        <v>426</v>
+      </c>
+      <c r="B237" t="s">
+        <v>425</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="238" s="2" spans="1:2">
       <c r="A238" s="1" t="s">
-        <v>353</v>
+        <v>427</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="239" s="2" spans="1:2">
       <c r="A239" s="1" t="s">
-        <v>354</v>
+        <v>428</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="240" s="2" spans="1:2">
       <c r="A240" s="1" t="s">
-        <v>355</v>
+        <v>429</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="241" s="2" spans="1:2">
       <c r="A241" s="1" t="s">
-        <v>356</v>
+        <v>430</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="242" s="2" spans="1:2">
       <c r="A242" s="1" t="s">
-        <v>357</v>
+        <v>431</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="243" s="2" spans="1:2">
       <c r="A243" s="1" t="s">
-        <v>358</v>
+        <v>432</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="244" s="2" spans="1:2">
       <c r="A244" s="1" t="s">
-        <v>359</v>
+        <v>433</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="245" s="2" spans="1:2">
       <c r="A245" s="1" t="s">
-        <v>360</v>
+        <v>434</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="246" s="2" spans="1:2">
       <c r="A246" s="1" t="s">
-        <v>360</v>
+        <v>434</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="247" s="2" spans="1:2">
       <c r="A247" s="1" t="s">
-        <v>361</v>
+        <v>435</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="248" s="2" spans="1:2">
       <c r="A248" s="1" t="s">
-        <v>362</v>
+        <v>436</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="249" s="2" spans="1:2">
       <c r="A249" s="1" t="s">
-        <v>363</v>
+        <v>437</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="250" s="2" spans="1:2">
       <c r="A250" s="1" t="s">
-        <v>364</v>
+        <v>438</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="251" s="2" spans="1:2">
       <c r="A251" s="1" t="s">
-        <v>365</v>
+        <v>439</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="252" s="2" spans="1:2">
       <c r="A252" s="1" t="s">
-        <v>366</v>
+        <v>440</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="253" s="2" spans="1:2">
       <c r="A253" s="1" t="s">
-        <v>367</v>
+        <v>441</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="254" s="2" spans="1:2">
       <c r="A254" s="1" t="s">
-        <v>368</v>
+        <v>442</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="255" s="2" spans="1:2">
       <c r="A255" s="1" t="s">
-        <v>368</v>
+        <v>442</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="256" s="2" spans="1:2">
       <c r="A256" s="1" t="s">
-        <v>369</v>
+        <v>443</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="257" s="2" spans="1:2">
       <c r="A257" s="1" t="s">
-        <v>369</v>
+        <v>443</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="258" s="2" spans="1:2">
       <c r="A258" s="1" t="s">
-        <v>369</v>
+        <v>443</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="259" s="2" spans="1:2">
       <c r="A259" s="1" t="s">
-        <v>369</v>
+        <v>443</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="260" s="2" spans="1:2">
       <c r="A260" s="1" t="s">
-        <v>369</v>
+        <v>443</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="261" s="2" spans="1:2">
       <c r="A261" s="1" t="s">
-        <v>370</v>
+        <v>444</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="262" s="2" spans="1:2">
       <c r="A262" s="1" t="s">
-        <v>371</v>
+        <v>445</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="263" s="2" spans="1:2">
       <c r="A263" s="1" t="s">
-        <v>372</v>
+        <v>446</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="264" s="2" spans="1:2">
       <c r="A264" s="1" t="s">
-        <v>372</v>
+        <v>446</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="265" s="2" spans="1:2">
       <c r="A265" s="1" t="s">
-        <v>373</v>
+        <v>447</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="266" s="2" spans="1:2">
       <c r="A266" s="1" t="s">
-        <v>374</v>
+        <v>448</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="267" s="2" spans="1:2">
       <c r="A267" s="1" t="s">
-        <v>375</v>
+        <v>449</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="268" s="2" spans="1:2">
       <c r="A268" s="1" t="s">
-        <v>376</v>
+        <v>450</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="269" s="2" spans="1:2">
       <c r="A269" s="1" t="s">
-        <v>376</v>
+        <v>450</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="270" s="2" spans="1:2">
       <c r="A270" s="1" t="s">
-        <v>377</v>
+        <v>451</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="271" s="2" spans="1:2">
       <c r="A271" s="1" t="s">
-        <v>378</v>
+        <v>452</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="272" s="2" spans="1:2">
       <c r="A272" s="1" t="s">
-        <v>379</v>
+        <v>453</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="273" s="2" spans="1:2">
       <c r="A273" s="1" t="s">
-        <v>379</v>
+        <v>453</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="274" s="2" spans="1:2">
       <c r="A274" s="1" t="s">
-        <v>380</v>
+        <v>454</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="275" s="2" spans="1:2">
       <c r="A275" s="1" t="s">
-        <v>381</v>
+        <v>455</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="276" s="2" spans="1:2">
       <c r="A276" s="1" t="s">
-        <v>382</v>
+        <v>456</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="277" s="2" spans="1:2">
       <c r="A277" s="1" t="s">
-        <v>383</v>
+        <v>457</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="278" s="2" spans="1:2">
       <c r="A278" s="1" t="s">
-        <v>384</v>
+        <v>458</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="279" s="2" spans="1:2">
       <c r="A279" s="1" t="s">
-        <v>385</v>
+        <v>459</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="280" s="2" spans="1:2">
       <c r="A280" s="1" t="s">
-        <v>386</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -3478,12 +3928,12 @@
   <sheetData>
     <row customHeight="1" ht="19" r="1" s="2" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>387</v>
+        <v>461</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="2" s="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>388</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>